<commit_message>
edited a few things
</commit_message>
<xml_diff>
--- a/Session 3 - Young Table/Answers/DS Lab report sheet.xlsx
+++ b/Session 3 - Young Table/Answers/DS Lab report sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varin\Downloads\Compressed\DS_3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varin\Documents\Data Structure Git\Data-Structure-Library-1402\Session 3 - Young Table\Answers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDB6227-A994-4D0F-BD24-D73C958A69B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785CC268-1F89-4461-8F02-B16573443A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t xml:space="preserve">Student Name </t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>milliseconds</t>
-  </si>
-  <si>
-    <t>محمدرضا امینی</t>
   </si>
   <si>
     <t>Windows 11</t>
@@ -220,22 +217,22 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,7 +454,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -477,12 +474,8 @@
       <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="9">
-        <v>402222020</v>
-      </c>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -497,13 +490,13 @@
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" ht="21.75" customHeight="1">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" ht="13.8" thickBot="1">
@@ -525,19 +518,19 @@
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="C6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="10">
+      <c r="D6" s="8">
         <v>8</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="8">
         <v>4.5999999999999996</v>
       </c>
       <c r="F6" s="3"/>
@@ -552,7 +545,7 @@
     </row>
     <row r="8" spans="1:6" ht="26.25" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -561,8 +554,8 @@
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" ht="22.5" customHeight="1">
-      <c r="A9" s="11" t="s">
-        <v>17</v>
+      <c r="A9" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -583,57 +576,57 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="22.5" customHeight="1">
-      <c r="A12" s="8">
+      <c r="A12" s="6">
         <v>250000</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="6">
         <v>852</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="22.5" customHeight="1">
-      <c r="A13" s="8">
+      <c r="A13" s="6">
         <v>360000</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="6">
         <v>766</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="22.5" customHeight="1">
-      <c r="A14" s="8">
+      <c r="A14" s="6">
         <v>490000</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="6">
         <v>1240</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="22.5" customHeight="1">
-      <c r="A15" s="8">
+      <c r="A15" s="6">
         <v>640000</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="6">
         <v>1833</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="22.5" customHeight="1">
-      <c r="A16" s="8">
+      <c r="A16" s="6">
         <v>1000000</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="6">
         <v>3575</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="6" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>